<commit_message>
* v1.2.1beta, 2025-01-07: Fix the color palette generation to avoid duplicate colors and make sure each author has a unique color.
</commit_message>
<xml_diff>
--- a/results/20250107_CDL_UMCU_Publications_collaborations.xlsx
+++ b/results/20250107_CDL_UMCU_Publications_collaborations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="144">
   <si>
     <t>Canonical Author 1</t>
   </si>
@@ -98,9 +98,6 @@
     <t>38639096</t>
   </si>
   <si>
-    <t>38695167</t>
-  </si>
-  <si>
     <t>39137621</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Single-Cell Gene-Regulatory Networks of Advanced Symptomatic Atherosclerosis.</t>
   </si>
   <si>
-    <t xml:space="preserve">IL-1beta Inhibition Partially Negates the Beneficial Effects of Diet-Induced </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tobacco smoking is associated with sex- and plaque-type specific upregulation of </t>
   </si>
   <si>
@@ -326,15 +320,9 @@
     <t>https://doi.org/10.1161/CIRCRESAHA.123.323184</t>
   </si>
   <si>
-    <t>https://doi.org/10.1161/ATVBAHA.124.320800</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1016/j.atherosclerosis.2024.118554</t>
   </si>
   <si>
-    <t>https://doi.org/10.1101/2023.10.13.562255.</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1186/s13287-023-03615-x</t>
   </si>
   <si>
@@ -395,13 +383,7 @@
     <t xml:space="preserve">Circ Res. 2024 May 24;134(11):1405-1423. doi: 10.1161/CIRCRESAHA.123.323184. Epub </t>
   </si>
   <si>
-    <t xml:space="preserve">Arterioscler Thromb Vasc Biol. 2024 Jun;44(6):1379-1392. doi: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Atherosclerosis. 2024 Oct;397:118554. doi: 10.1016/j.atherosclerosis.2024.118554. </t>
-  </si>
-  <si>
-    <t>bioRxiv. 2023 Oct 14:2023.10.13.562255. doi:</t>
   </si>
   <si>
     <t>Stem Cell Res Ther. 2024 Jan 17;15(1):19. doi: 10.1186/s13287-023-03615-x.</t>
@@ -835,7 +817,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -881,22 +863,22 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -910,22 +892,22 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -939,22 +921,22 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -968,22 +950,22 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -997,22 +979,22 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1026,22 +1008,22 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1055,22 +1037,22 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1084,22 +1066,22 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1113,22 +1095,22 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1142,22 +1124,22 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1171,22 +1153,22 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1200,22 +1182,22 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1229,22 +1211,22 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1258,22 +1240,22 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1287,22 +1269,22 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1316,22 +1298,22 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1345,22 +1327,22 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1374,22 +1356,22 @@
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1403,22 +1385,22 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1432,22 +1414,22 @@
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1455,13 +1437,13 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
         <v>45</v>
@@ -1470,39 +1452,39 @@
         <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I22" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I23" t="s">
         <v>122</v>
@@ -1513,57 +1495,57 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I25" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1571,54 +1553,54 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
         <v>43</v>
       </c>
-      <c r="E26" t="s">
-        <v>49</v>
-      </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G27" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I27" t="s">
         <v>123</v>
@@ -1626,31 +1608,31 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I28" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1658,57 +1640,57 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="I29" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
         <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1716,57 +1698,57 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I31" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I32" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1774,33 +1756,33 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -1809,27 +1791,27 @@
         <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I34" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -1838,77 +1820,77 @@
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I35" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I36" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
         <v>9</v>
       </c>
-      <c r="B37" t="s">
-        <v>17</v>
-      </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F37" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G37" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I37" t="s">
         <v>121</v>
@@ -1916,31 +1898,31 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F38" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G38" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I38" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1948,13 +1930,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" t="s">
         <v>48</v>
@@ -1966,39 +1948,39 @@
         <v>80</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I40" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2006,13 +1988,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s">
         <v>49</v>
@@ -2024,39 +2006,39 @@
         <v>82</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>104</v>
       </c>
       <c r="I42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2067,25 +2049,25 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I43" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2099,7 +2081,7 @@
         <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E44" t="s">
         <v>51</v>
@@ -2108,13 +2090,13 @@
         <v>67</v>
       </c>
       <c r="G44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2128,36 +2110,36 @@
         <v>29</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I45" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
         <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E46" t="s">
         <v>52</v>
@@ -2166,42 +2148,42 @@
         <v>68</v>
       </c>
       <c r="G46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I46" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G47" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2212,25 +2194,25 @@
         <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G48" t="s">
         <v>87</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I48" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2241,39 +2223,39 @@
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G49" t="s">
         <v>88</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I49" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E50" t="s">
         <v>55</v>
@@ -2285,10 +2267,10 @@
         <v>89</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I50" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2302,51 +2284,51 @@
         <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I51" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I52" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2360,7 +2342,7 @@
         <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E53" t="s">
         <v>56</v>
@@ -2369,42 +2351,42 @@
         <v>72</v>
       </c>
       <c r="G53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I53" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G54" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I54" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2415,25 +2397,25 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G55" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I55" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2441,28 +2423,28 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G56" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I56" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2476,51 +2458,51 @@
         <v>36</v>
       </c>
       <c r="D57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E57" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I57" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G58" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I58" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2534,7 +2516,7 @@
         <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E59" t="s">
         <v>56</v>
@@ -2543,129 +2525,129 @@
         <v>72</v>
       </c>
       <c r="G59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I59" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E60" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G60" t="s">
         <v>91</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I60" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E61" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F61" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G61" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="I61" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F62" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G62" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="I62" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C63" t="s">
         <v>25</v>
       </c>
       <c r="D63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2673,57 +2655,57 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E64" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F64" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G64" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I64" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
       </c>
       <c r="C65" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E65" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F65" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G65" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I65" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2731,33 +2713,33 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C66" t="s">
         <v>23</v>
       </c>
       <c r="D66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I66" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
@@ -2766,27 +2748,27 @@
         <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I67" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
         <v>17</v>
@@ -2795,109 +2777,109 @@
         <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I68" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C69" t="s">
         <v>23</v>
       </c>
       <c r="D69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I69" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
         <v>9</v>
       </c>
-      <c r="B70" t="s">
-        <v>17</v>
-      </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E70" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F70" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G70" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I70" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="B71" t="s">
-        <v>17</v>
-      </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E71" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F71" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G71" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I71" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2911,631 +2893,515 @@
         <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E72" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F72" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I72" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E73" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F73" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G73" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I73" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E74" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F74" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G74" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I74" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E75" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F75" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G75" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I75" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D76" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E76" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F76" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G76" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I76" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C77" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D77" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E77" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F77" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G77" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I77" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E78" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F78" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G78" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I78" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E79" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G79" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I79" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C80" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E80" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F80" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G80" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I80" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F81" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G81" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="I81" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E82" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F82" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G82" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I82" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E83" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G83" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>112</v>
       </c>
       <c r="I83" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D84" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E84" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F84" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G84" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I84" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C85" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D85" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E85" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F85" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G85" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I85" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C86" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E86" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F86" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G86" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I86" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C87" t="s">
         <v>39</v>
       </c>
       <c r="D87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E87" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F87" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I87" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C88" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E88" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F88" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G88" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>114</v>
       </c>
       <c r="I88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C89" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E89" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F89" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G89" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I89" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" t="s">
-        <v>15</v>
-      </c>
-      <c r="B90" t="s">
-        <v>13</v>
-      </c>
-      <c r="C90" t="s">
-        <v>37</v>
-      </c>
-      <c r="D90" t="s">
-        <v>43</v>
-      </c>
-      <c r="E90" t="s">
-        <v>56</v>
-      </c>
-      <c r="F90" t="s">
-        <v>72</v>
-      </c>
-      <c r="G90" t="s">
-        <v>91</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I90" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" t="s">
-        <v>16</v>
-      </c>
-      <c r="B91" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" t="s">
-        <v>40</v>
-      </c>
-      <c r="D91" t="s">
-        <v>43</v>
-      </c>
-      <c r="E91" t="s">
-        <v>58</v>
-      </c>
-      <c r="F91" t="s">
-        <v>74</v>
-      </c>
-      <c r="G91" t="s">
-        <v>94</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I91" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" t="s">
-        <v>16</v>
-      </c>
-      <c r="B92" t="s">
-        <v>21</v>
-      </c>
-      <c r="C92" t="s">
-        <v>41</v>
-      </c>
-      <c r="D92" t="s">
-        <v>43</v>
-      </c>
-      <c r="E92" t="s">
-        <v>59</v>
-      </c>
-      <c r="F92" t="s">
-        <v>75</v>
-      </c>
-      <c r="G92" t="s">
-        <v>95</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I92" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" t="s">
-        <v>16</v>
-      </c>
-      <c r="B93" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93" t="s">
-        <v>42</v>
-      </c>
-      <c r="D93" t="s">
-        <v>43</v>
-      </c>
-      <c r="E93" t="s">
-        <v>58</v>
-      </c>
-      <c r="F93" t="s">
-        <v>74</v>
-      </c>
-      <c r="G93" t="s">
-        <v>96</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I93" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3628,10 +3494,6 @@
     <hyperlink ref="H87" r:id="rId86"/>
     <hyperlink ref="H88" r:id="rId87"/>
     <hyperlink ref="H89" r:id="rId88"/>
-    <hyperlink ref="H90" r:id="rId89"/>
-    <hyperlink ref="H91" r:id="rId90"/>
-    <hyperlink ref="H92" r:id="rId91"/>
-    <hyperlink ref="H93" r:id="rId92"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3647,7 +3509,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3673,782 +3535,782 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H22" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H26" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H27" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H28" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H29" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H30" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H31" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>